<commit_message>
update toàn bộ file
</commit_message>
<xml_diff>
--- a/public/files/DS_BenhNhan.xlsx
+++ b/public/files/DS_BenhNhan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huyan\OneDrive\Máy tính\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B92733B7-D00C-47A5-97C9-5C93838B3C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187AF0D4-9311-4C7D-81E3-9EFFC3209DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6B3951E2-CA38-424D-845E-A2572D9B61AA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6B3951E2-CA38-424D-845E-A2572D9B61AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Tên Bệnh Nhân</t>
   </si>
   <si>
-    <t>Tuổi</t>
-  </si>
-  <si>
     <t>Điện thoại</t>
-  </si>
-  <si>
-    <t>Ngày tháng năm sinh</t>
   </si>
   <si>
     <t>Giới Tính</t>
@@ -47,12 +41,15 @@
   <si>
     <t>Ngày nhập</t>
   </si>
+  <si>
+    <t>Năm sinh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +74,29 @@
       <family val="1"/>
       <charset val="163"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -117,21 +137,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -443,48 +487,742 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F28839-B592-4EC0-8711-BC61A6403306}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="68.25" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="37.875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="13.375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="23.625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="40.75" style="11" customWidth="1"/>
+    <col min="6" max="6" width="20.25" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="2"/>
+      <c r="B50" s="3"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="3"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="3"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="2"/>
+      <c r="B54" s="3"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="2"/>
+      <c r="B55" s="3"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="2"/>
+      <c r="B56" s="3"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="2"/>
+      <c r="B57" s="3"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="2"/>
+      <c r="B58" s="3"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="2"/>
+      <c r="B59" s="3"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="7"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="2"/>
+      <c r="B60" s="3"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="2"/>
+      <c r="B61" s="3"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="2"/>
+      <c r="B62" s="3"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="2"/>
+      <c r="B63" s="3"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="2"/>
+      <c r="B64" s="3"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="2"/>
+      <c r="B65" s="3"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="2"/>
+      <c r="B66" s="3"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="7"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="2"/>
+      <c r="B67" s="3"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="2"/>
+      <c r="B68" s="3"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="7"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="2"/>
+      <c r="B69" s="3"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="2"/>
+      <c r="B70" s="3"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="2"/>
+      <c r="B71" s="3"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="7"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="2"/>
+      <c r="B72" s="3"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="2"/>
+      <c r="B73" s="3"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="7"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="2"/>
+      <c r="B74" s="3"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="7"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="2"/>
+      <c r="B75" s="3"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="2"/>
+      <c r="B76" s="3"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="2"/>
+      <c r="B77" s="3"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="2"/>
+      <c r="B78" s="3"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="2"/>
+      <c r="B79" s="3"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="2"/>
+      <c r="B80" s="3"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="2"/>
+      <c r="B81" s="3"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="7"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="2"/>
+      <c r="B82" s="3"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="7"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="2"/>
+      <c r="B83" s="3"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="7"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="2"/>
+      <c r="B84" s="3"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="7"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="2"/>
+      <c r="B85" s="3"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="7"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="2"/>
+      <c r="B86" s="3"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="7"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="2"/>
+      <c r="B87" s="3"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="7"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="2"/>
+      <c r="B88" s="3"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="7"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="2"/>
+      <c r="B89" s="3"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="7"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="2"/>
+      <c r="B90" s="3"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="7"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="2"/>
+      <c r="B91" s="3"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="7"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="2"/>
+      <c r="B92" s="3"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="7"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="2"/>
+      <c r="B93" s="3"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="7"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="2"/>
+      <c r="B94" s="3"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="7"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" s="2"/>
+      <c r="B95" s="3"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="7"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" s="2"/>
+      <c r="B96" s="3"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="7"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="2"/>
+      <c r="B97" s="3"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="7"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="2"/>
+      <c r="B98" s="3"/>
+      <c r="E98" s="4"/>
+      <c r="F98" s="7"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="2"/>
+      <c r="B99" s="3"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="7"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" s="2"/>
+      <c r="B100" s="3"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="7"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="2"/>
+      <c r="B101" s="3"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="7"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" s="2"/>
+      <c r="B102" s="3"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="7"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="2"/>
+      <c r="B103" s="3"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="7"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="2"/>
+      <c r="B104" s="3"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="7"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" s="2"/>
+      <c r="B105" s="3"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="7"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="2"/>
+      <c r="B106" s="3"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="7"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="2"/>
+      <c r="B107" s="3"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="7"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="2"/>
+      <c r="B108" s="3"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="7"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="2"/>
+      <c r="B109" s="3"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="7"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="2"/>
+      <c r="B110" s="3"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="7"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="2"/>
+      <c r="B111" s="3"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>